<commit_message>
- checked column with input-variables to avoid space character which could cause errors - added respective questions for the meeting with Benedict in comment column
</commit_message>
<xml_diff>
--- a/Franzi/DPE_KARMEN_FRANZI.xlsx
+++ b/Franzi/DPE_KARMEN_FRANZI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\Franzi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3CAE1E6-3E86-47BF-A09B-1473F5D65862}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F78D9D5-1EC0-48DD-951D-B5E7061C5864}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1095" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="331">
   <si>
     <t>index</t>
   </si>
@@ -952,62 +952,67 @@
     <t>Zu geringe Anzahl an Konsumenten für Berechnung via NCI-Methode (Recall1: n=2; Recall2: n=3) </t>
   </si>
   <si>
-    <t>Fermented_milk_NCI </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Would it be possible to calculate % of cheese curd intake from the group Milc07_2? </t>
-  </si>
-  <si>
     <t xml:space="preserve">Would it be possible to calculate % of cheese intake from the group Milc07_2? </t>
   </si>
   <si>
-    <t>Flours_milled_prod_NCI </t>
-  </si>
-  <si>
     <t>Pasta_rice_NCI</t>
   </si>
   <si>
-    <t>Bread_NCI </t>
-  </si>
-  <si>
-    <t>Crispbread_NCI </t>
-  </si>
-  <si>
     <t>Breakfast_cereals_NCI</t>
   </si>
   <si>
     <t>Crackers_NCI </t>
   </si>
   <si>
-    <t>Fine_bakery_NCI </t>
-  </si>
-  <si>
     <t>Eier_sum_NCI</t>
   </si>
   <si>
-    <t>veg_fatsoils_NCI </t>
-  </si>
-  <si>
-    <t>Butter_NCI </t>
-  </si>
-  <si>
-    <t>Marg_Streichf_NCI </t>
-  </si>
-  <si>
-    <t>Animal_fatsoils_NCI </t>
-  </si>
-  <si>
-    <t>Cakes_NCI </t>
-  </si>
-  <si>
-    <t>Veg_products_NCI </t>
-  </si>
-  <si>
-    <t>Soyproducts_NCI </t>
-  </si>
-  <si>
-    <t>Getr15_12; 
-Getr15_13</t>
+    <t>Fermented_milk_NCI</t>
+  </si>
+  <si>
+    <t>Flours_milled_prod_NCI</t>
+  </si>
+  <si>
+    <t>Bread_NCI</t>
+  </si>
+  <si>
+    <t>Crispbread_NCI</t>
+  </si>
+  <si>
+    <t>Fine_bakery_NCI</t>
+  </si>
+  <si>
+    <t>veg_fatsoils_NCI</t>
+  </si>
+  <si>
+    <t>Butter_NCI</t>
+  </si>
+  <si>
+    <t>Marg_Streichf_NCI</t>
+  </si>
+  <si>
+    <t>Animal_fatsoils_NCI</t>
+  </si>
+  <si>
+    <t>Cakes_NCI</t>
+  </si>
+  <si>
+    <t>Getr15_12; Getr15_13</t>
+  </si>
+  <si>
+    <t>Veg_products_NCI</t>
+  </si>
+  <si>
+    <t>Soyproducts_NCI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Would it be possible to calculate % of cheese curd, quark and cottage intake from the group Milc07_2? </t>
+  </si>
+  <si>
+    <t>Do you know the proportion of coffee drinkers? Does 50% make sense?</t>
+  </si>
+  <si>
+    <t>Do you know the proportion of tea drinkers? Does 50% make sense?</t>
   </si>
 </sst>
 </file>
@@ -1069,8 +1074,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1108,7 +1113,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1147,10 +1152,13 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1494,7 +1502,7 @@
   <dimension ref="A1:K121"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I125" sqref="I125"/>
+      <selection activeCell="B89" sqref="B89:B90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1547,6 +1555,9 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -1579,6 +1590,9 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -1609,6 +1623,9 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
       <c r="B4" t="s">
         <v>16</v>
       </c>
@@ -1639,6 +1656,9 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
       <c r="B5" t="s">
         <v>18</v>
       </c>
@@ -1669,6 +1689,9 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
       <c r="B6" t="s">
         <v>20</v>
       </c>
@@ -1699,6 +1722,9 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
       <c r="B7" t="s">
         <v>22</v>
       </c>
@@ -1729,6 +1755,9 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
       <c r="B8" t="s">
         <v>24</v>
       </c>
@@ -1759,6 +1788,9 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
       <c r="B9" t="s">
         <v>26</v>
       </c>
@@ -1789,6 +1821,9 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
       <c r="B10" t="s">
         <v>28</v>
       </c>
@@ -1819,6 +1854,9 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
       <c r="B11" t="s">
         <v>30</v>
       </c>
@@ -1849,6 +1887,9 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
       <c r="B12" t="s">
         <v>32</v>
       </c>
@@ -1879,6 +1920,9 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
       <c r="B13" t="s">
         <v>34</v>
       </c>
@@ -1909,6 +1953,9 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
       <c r="B14" t="s">
         <v>36</v>
       </c>
@@ -1939,6 +1986,9 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
       <c r="B15" t="s">
         <v>38</v>
       </c>
@@ -1969,6 +2019,9 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
       <c r="B16" t="s">
         <v>40</v>
       </c>
@@ -1998,7 +2051,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
       <c r="B17" t="s">
         <v>42</v>
       </c>
@@ -2028,7 +2084,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
       <c r="B18" t="s">
         <v>44</v>
       </c>
@@ -2058,7 +2117,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
       <c r="B19" t="s">
         <v>46</v>
       </c>
@@ -2088,7 +2150,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
       <c r="B20" t="s">
         <v>48</v>
       </c>
@@ -2118,7 +2183,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
       <c r="B21" t="s">
         <v>50</v>
       </c>
@@ -2148,7 +2216,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
       <c r="B22" t="s">
         <v>52</v>
       </c>
@@ -2178,7 +2249,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
       <c r="B23" t="s">
         <v>54</v>
       </c>
@@ -2197,10 +2271,10 @@
       <c r="G23" s="14" t="s">
         <v>295</v>
       </c>
-      <c r="H23" s="4" t="s">
+      <c r="H23" s="22" t="s">
         <v>307</v>
       </c>
-      <c r="I23" s="4" t="s">
+      <c r="I23" s="22" t="s">
         <v>308</v>
       </c>
       <c r="J23" s="14" t="s">
@@ -2210,7 +2284,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
       <c r="B24" t="s">
         <v>56</v>
       </c>
@@ -2242,7 +2319,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
       <c r="B25" t="s">
         <v>58</v>
       </c>
@@ -2256,7 +2336,7 @@
         <v>253</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="G25" s="14" t="s">
         <v>288</v>
@@ -2272,7 +2352,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
       <c r="B26" t="s">
         <v>60</v>
       </c>
@@ -2285,17 +2368,17 @@
       <c r="E26" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="F26" s="20" t="s">
+      <c r="F26" s="21" t="s">
         <v>262</v>
       </c>
       <c r="G26" s="14" t="s">
         <v>295</v>
       </c>
-      <c r="H26" s="4" t="s">
+      <c r="H26" s="22" t="s">
         <v>307</v>
       </c>
-      <c r="I26" s="4" t="s">
-        <v>311</v>
+      <c r="I26" s="22" t="s">
+        <v>328</v>
       </c>
       <c r="J26" s="14" t="s">
         <v>292</v>
@@ -2304,7 +2387,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
       <c r="B27" t="s">
         <v>62</v>
       </c>
@@ -2323,11 +2409,11 @@
       <c r="G27" s="14" t="s">
         <v>295</v>
       </c>
-      <c r="H27" s="4" t="s">
+      <c r="H27" s="22" t="s">
         <v>307</v>
       </c>
-      <c r="I27" s="4" t="s">
-        <v>312</v>
+      <c r="I27" s="22" t="s">
+        <v>310</v>
       </c>
       <c r="J27" s="14" t="s">
         <v>292</v>
@@ -2336,7 +2422,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
       <c r="B28" t="s">
         <v>64</v>
       </c>
@@ -2366,7 +2455,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
       <c r="B29" t="s">
         <v>66</v>
       </c>
@@ -2396,7 +2488,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
       <c r="B30" t="s">
         <v>68</v>
       </c>
@@ -2426,7 +2521,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
       <c r="B31" t="s">
         <v>70</v>
       </c>
@@ -2456,7 +2554,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
       <c r="B32" t="s">
         <v>72</v>
       </c>
@@ -2486,7 +2587,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
       <c r="B33" t="s">
         <v>74</v>
       </c>
@@ -2516,7 +2620,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
       <c r="B34" t="s">
         <v>76</v>
       </c>
@@ -2530,7 +2637,7 @@
         <v>253</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>288</v>
@@ -2546,7 +2653,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
       <c r="B35" t="s">
         <v>78</v>
       </c>
@@ -2560,7 +2670,7 @@
         <v>253</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>288</v>
@@ -2576,7 +2686,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
       <c r="B36" t="s">
         <v>80</v>
       </c>
@@ -2606,7 +2719,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
       <c r="B37" t="s">
         <v>82</v>
       </c>
@@ -2620,7 +2736,7 @@
         <v>253</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="G37" s="14" t="s">
         <v>288</v>
@@ -2636,7 +2752,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
       <c r="B38" t="s">
         <v>84</v>
       </c>
@@ -2650,7 +2769,7 @@
         <v>253</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="G38" s="14" t="s">
         <v>288</v>
@@ -2666,7 +2785,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
       <c r="B39" t="s">
         <v>86</v>
       </c>
@@ -2680,7 +2802,7 @@
         <v>253</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="G39" s="14" t="s">
         <v>288</v>
@@ -2696,7 +2818,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
       <c r="B40" t="s">
         <v>88</v>
       </c>
@@ -2710,7 +2835,7 @@
         <v>253</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="G40" s="14" t="s">
         <v>288</v>
@@ -2726,7 +2851,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
       <c r="B41" t="s">
         <v>90</v>
       </c>
@@ -2756,7 +2884,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
       <c r="B42" t="s">
         <v>92</v>
       </c>
@@ -2786,7 +2917,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
       <c r="B43" t="s">
         <v>94</v>
       </c>
@@ -2816,7 +2950,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
       <c r="B44" t="s">
         <v>96</v>
       </c>
@@ -2846,7 +2983,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
       <c r="B45" t="s">
         <v>98</v>
       </c>
@@ -2876,7 +3016,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
       <c r="B46" t="s">
         <v>100</v>
       </c>
@@ -2906,7 +3049,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
       <c r="B47" t="s">
         <v>102</v>
       </c>
@@ -2936,7 +3082,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
       <c r="B48" t="s">
         <v>104</v>
       </c>
@@ -2966,7 +3115,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
       <c r="B49" t="s">
         <v>106</v>
       </c>
@@ -2996,7 +3148,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
       <c r="B50" t="s">
         <v>108</v>
       </c>
@@ -3026,7 +3181,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
       <c r="B51" t="s">
         <v>110</v>
       </c>
@@ -3056,7 +3214,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
       <c r="B52" t="s">
         <v>112</v>
       </c>
@@ -3086,7 +3247,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
       <c r="B53" t="s">
         <v>114</v>
       </c>
@@ -3116,7 +3280,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
       <c r="B54" t="s">
         <v>116</v>
       </c>
@@ -3146,7 +3313,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
       <c r="B55" t="s">
         <v>118</v>
       </c>
@@ -3176,7 +3346,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
       <c r="B56" t="s">
         <v>120</v>
       </c>
@@ -3206,7 +3379,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
       <c r="B57" t="s">
         <v>122</v>
       </c>
@@ -3236,7 +3412,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
       <c r="B58" t="s">
         <v>124</v>
       </c>
@@ -3255,7 +3434,9 @@
       <c r="G58" s="10" t="s">
         <v>288</v>
       </c>
-      <c r="H58" s="9"/>
+      <c r="H58" s="14" t="s">
+        <v>288</v>
+      </c>
       <c r="I58" s="9"/>
       <c r="J58" s="10" t="s">
         <v>292</v>
@@ -3264,7 +3445,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
       <c r="B59" t="s">
         <v>126</v>
       </c>
@@ -3294,7 +3478,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
       <c r="B60" t="s">
         <v>128</v>
       </c>
@@ -3324,7 +3511,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
       <c r="B61" t="s">
         <v>130</v>
       </c>
@@ -3354,7 +3544,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
       <c r="B62" t="s">
         <v>132</v>
       </c>
@@ -3384,7 +3577,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="63" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
       <c r="B63" t="s">
         <v>134</v>
       </c>
@@ -3414,7 +3610,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="64" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
       <c r="B64" t="s">
         <v>136</v>
       </c>
@@ -3428,7 +3627,7 @@
         <v>253</v>
       </c>
       <c r="F64" s="13" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="G64" s="10" t="s">
         <v>288</v>
@@ -3444,7 +3643,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="65" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
       <c r="B65" t="s">
         <v>138</v>
       </c>
@@ -3474,7 +3676,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="66" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
       <c r="B66" t="s">
         <v>140</v>
       </c>
@@ -3504,7 +3709,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
       <c r="B67" t="s">
         <v>142</v>
       </c>
@@ -3518,7 +3726,7 @@
         <v>253</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G67" s="14" t="s">
         <v>288</v>
@@ -3534,7 +3742,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>67</v>
+      </c>
       <c r="B68" t="s">
         <v>144</v>
       </c>
@@ -3548,7 +3759,7 @@
         <v>253</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G68" s="14" t="s">
         <v>288</v>
@@ -3564,7 +3775,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="69" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>68</v>
+      </c>
       <c r="B69" t="s">
         <v>146</v>
       </c>
@@ -3578,7 +3792,7 @@
         <v>253</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G69" s="14" t="s">
         <v>288</v>
@@ -3594,7 +3808,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="70" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
       <c r="B70" t="s">
         <v>148</v>
       </c>
@@ -3624,7 +3841,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="71" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>70</v>
+      </c>
       <c r="B71" t="s">
         <v>150</v>
       </c>
@@ -3654,7 +3874,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="72" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>71</v>
+      </c>
       <c r="B72" t="s">
         <v>152</v>
       </c>
@@ -3668,7 +3891,7 @@
         <v>253</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G72" s="14" t="s">
         <v>288</v>
@@ -3684,7 +3907,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="73" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>72</v>
+      </c>
       <c r="B73" t="s">
         <v>154</v>
       </c>
@@ -3714,7 +3940,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="74" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>73</v>
+      </c>
       <c r="B74" t="s">
         <v>156</v>
       </c>
@@ -3744,7 +3973,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="75" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>74</v>
+      </c>
       <c r="B75" t="s">
         <v>158</v>
       </c>
@@ -3774,7 +4006,10 @@
         <v>296</v>
       </c>
     </row>
-    <row r="76" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>75</v>
+      </c>
       <c r="B76" t="s">
         <v>160</v>
       </c>
@@ -3804,7 +4039,10 @@
         <v>296</v>
       </c>
     </row>
-    <row r="77" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>76</v>
+      </c>
       <c r="B77" t="s">
         <v>162</v>
       </c>
@@ -3834,7 +4072,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="78" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>77</v>
+      </c>
       <c r="B78" t="s">
         <v>164</v>
       </c>
@@ -3864,7 +4105,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="79" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>78</v>
+      </c>
       <c r="B79" t="s">
         <v>166</v>
       </c>
@@ -3894,7 +4138,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="80" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>79</v>
+      </c>
       <c r="B80" t="s">
         <v>168</v>
       </c>
@@ -3924,7 +4171,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="81" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>80</v>
+      </c>
       <c r="B81" t="s">
         <v>170</v>
       </c>
@@ -3954,7 +4204,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="82" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>81</v>
+      </c>
       <c r="B82" t="s">
         <v>172</v>
       </c>
@@ -3968,7 +4221,7 @@
         <v>253</v>
       </c>
       <c r="F82" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G82" s="10" t="s">
         <v>288</v>
@@ -3984,7 +4237,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="83" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>82</v>
+      </c>
       <c r="B83" t="s">
         <v>174</v>
       </c>
@@ -4014,7 +4270,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="84" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>83</v>
+      </c>
       <c r="B84" t="s">
         <v>176</v>
       </c>
@@ -4044,7 +4303,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="85" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>84</v>
+      </c>
       <c r="B85" t="s">
         <v>178</v>
       </c>
@@ -4074,7 +4336,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="86" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>85</v>
+      </c>
       <c r="B86" t="s">
         <v>180</v>
       </c>
@@ -4104,7 +4369,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="87" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>86</v>
+      </c>
       <c r="B87" t="s">
         <v>182</v>
       </c>
@@ -4134,7 +4402,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="88" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>87</v>
+      </c>
       <c r="B88" t="s">
         <v>184</v>
       </c>
@@ -4147,8 +4418,8 @@
       <c r="E88" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="F88" s="21" t="s">
-        <v>328</v>
+      <c r="F88" s="20" t="s">
+        <v>325</v>
       </c>
       <c r="G88" s="14" t="s">
         <v>295</v>
@@ -4164,7 +4435,10 @@
         <v>300</v>
       </c>
     </row>
-    <row r="89" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>88</v>
+      </c>
       <c r="B89" t="s">
         <v>186</v>
       </c>
@@ -4183,10 +4457,12 @@
       <c r="G89" s="14" t="s">
         <v>295</v>
       </c>
-      <c r="H89" s="4" t="s">
+      <c r="H89" s="22" t="s">
         <v>301</v>
       </c>
-      <c r="I89" s="4"/>
+      <c r="I89" s="22" t="s">
+        <v>329</v>
+      </c>
       <c r="J89" s="14" t="s">
         <v>298</v>
       </c>
@@ -4194,7 +4470,10 @@
         <v>296</v>
       </c>
     </row>
-    <row r="90" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>89</v>
+      </c>
       <c r="B90" t="s">
         <v>188</v>
       </c>
@@ -4213,10 +4492,12 @@
       <c r="G90" s="14" t="s">
         <v>295</v>
       </c>
-      <c r="H90" s="4" t="s">
+      <c r="H90" s="22" t="s">
         <v>301</v>
       </c>
-      <c r="I90" s="4"/>
+      <c r="I90" s="22" t="s">
+        <v>330</v>
+      </c>
       <c r="J90" s="14" t="s">
         <v>298</v>
       </c>
@@ -4224,7 +4505,10 @@
         <v>296</v>
       </c>
     </row>
-    <row r="91" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>90</v>
+      </c>
       <c r="B91" t="s">
         <v>190</v>
       </c>
@@ -4254,7 +4538,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="92" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>91</v>
+      </c>
       <c r="B92" t="s">
         <v>192</v>
       </c>
@@ -4284,7 +4571,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="93" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>92</v>
+      </c>
       <c r="B93" t="s">
         <v>194</v>
       </c>
@@ -4314,7 +4604,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="94" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>93</v>
+      </c>
       <c r="B94" t="s">
         <v>196</v>
       </c>
@@ -4344,7 +4637,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="95" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>94</v>
+      </c>
       <c r="B95" t="s">
         <v>198</v>
       </c>
@@ -4374,7 +4670,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="96" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>95</v>
+      </c>
       <c r="B96" t="s">
         <v>200</v>
       </c>
@@ -4404,7 +4703,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="97" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>96</v>
+      </c>
       <c r="B97" t="s">
         <v>202</v>
       </c>
@@ -4434,7 +4736,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="98" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>97</v>
+      </c>
       <c r="B98" t="s">
         <v>204</v>
       </c>
@@ -4464,7 +4769,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="99" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>98</v>
+      </c>
       <c r="B99" t="s">
         <v>206</v>
       </c>
@@ -4494,7 +4802,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="100" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>99</v>
+      </c>
       <c r="B100" t="s">
         <v>208</v>
       </c>
@@ -4524,7 +4835,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="101" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>100</v>
+      </c>
       <c r="B101" t="s">
         <v>210</v>
       </c>
@@ -4554,7 +4868,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="102" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>101</v>
+      </c>
       <c r="B102" t="s">
         <v>212</v>
       </c>
@@ -4584,7 +4901,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="103" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>102</v>
+      </c>
       <c r="B103" t="s">
         <v>214</v>
       </c>
@@ -4614,7 +4934,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="104" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>103</v>
+      </c>
       <c r="B104" t="s">
         <v>216</v>
       </c>
@@ -4644,7 +4967,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="105" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>104</v>
+      </c>
       <c r="B105" t="s">
         <v>218</v>
       </c>
@@ -4674,7 +5000,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="106" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>105</v>
+      </c>
       <c r="B106" t="s">
         <v>220</v>
       </c>
@@ -4704,7 +5033,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="107" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>106</v>
+      </c>
       <c r="B107" t="s">
         <v>222</v>
       </c>
@@ -4734,7 +5066,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="108" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>107</v>
+      </c>
       <c r="B108" t="s">
         <v>224</v>
       </c>
@@ -4764,7 +5099,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="109" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>108</v>
+      </c>
       <c r="B109" t="s">
         <v>226</v>
       </c>
@@ -4794,7 +5132,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="110" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>109</v>
+      </c>
       <c r="B110" t="s">
         <v>228</v>
       </c>
@@ -4824,7 +5165,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="111" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>110</v>
+      </c>
       <c r="B111" t="s">
         <v>230</v>
       </c>
@@ -4854,7 +5198,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="112" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>111</v>
+      </c>
       <c r="B112" t="s">
         <v>232</v>
       </c>
@@ -4884,7 +5231,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="113" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>112</v>
+      </c>
       <c r="B113" t="s">
         <v>234</v>
       </c>
@@ -4914,7 +5264,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="114" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>113</v>
+      </c>
       <c r="B114" t="s">
         <v>236</v>
       </c>
@@ -4944,7 +5297,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="115" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>114</v>
+      </c>
       <c r="B115" t="s">
         <v>238</v>
       </c>
@@ -4974,7 +5330,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="116" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>115</v>
+      </c>
       <c r="B116" t="s">
         <v>240</v>
       </c>
@@ -5004,7 +5363,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="117" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>116</v>
+      </c>
       <c r="B117" t="s">
         <v>242</v>
       </c>
@@ -5034,7 +5396,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="118" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>117</v>
+      </c>
       <c r="B118" t="s">
         <v>244</v>
       </c>
@@ -5064,7 +5429,10 @@
         <v>293</v>
       </c>
     </row>
-    <row r="119" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>118</v>
+      </c>
       <c r="B119" t="s">
         <v>246</v>
       </c>
@@ -5094,7 +5462,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="120" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>119</v>
+      </c>
       <c r="B120" t="s">
         <v>248</v>
       </c>
@@ -5124,7 +5495,10 @@
         <v>294</v>
       </c>
     </row>
-    <row r="121" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>120</v>
+      </c>
       <c r="B121" t="s">
         <v>250</v>
       </c>

</xml_diff>